<commit_message>
reorganized hydro main functions; began working in the initial condition
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\fc_hydro_kalimantan_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DA7ABE-DBFD-4C81-8945-37C4583BB777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3031DEB4-0CBA-473F-9451-0D975E01515E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="3285" windowWidth="19785" windowHeight="13305" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1695" yWindow="3075" windowWidth="26505" windowHeight="13125" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t># Pointers to input and output files. Paths must be relative to daily_map.py script.</t>
   </si>
@@ -95,6 +95,12 @@
   </si>
   <si>
     <t xml:space="preserve">daily P - ET in meters for each weather station </t>
+  </si>
+  <si>
+    <t>data/reprojected_dipwells.gpkg</t>
+  </si>
+  <si>
+    <t>sensor_locations</t>
   </si>
 </sst>
 </file>
@@ -464,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,6 +594,14 @@
         <v>14</v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
produced initial condition dipwell locations and measurements
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\fc_hydro_kalimantan_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3031DEB4-0CBA-473F-9451-0D975E01515E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB79FD3-A5B2-422D-BC9B-03D3175EAD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1695" yWindow="3075" windowWidth="26505" windowHeight="13125" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t># Pointers to input and output files. Paths must be relative to daily_map.py script.</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>sensor_locations</t>
+  </si>
+  <si>
+    <t>initial_dipwell_measurements</t>
+  </si>
+  <si>
+    <t>initial_condition/initial_day_dipwell_coords_and_measurements.csv</t>
   </si>
 </sst>
 </file>
@@ -470,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,6 +608,14 @@
         <v>25</v>
       </c>
     </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
working calibration: comparing modelled to measured
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\fc_hydro_kalimantan_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB79FD3-A5B2-422D-BC9B-03D3175EAD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBAA09A-416F-4EA3-BAA6-A369C4AD14BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="3075" windowWidth="26505" windowHeight="13125" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t># Pointers to input and output files. Paths must be relative to daily_map.py script.</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>initial_condition/initial_day_dipwell_coords_and_measurements.csv</t>
+  </si>
+  <si>
+    <t>dipwell_measurements</t>
+  </si>
+  <si>
+    <t>data/dipwell_data_from_first_rainfall_record.csv</t>
   </si>
 </sst>
 </file>
@@ -476,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,6 +622,14 @@
         <v>28</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
worked on gmsh script for smaller mesh sizes in canals
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\fc_hydro_kalimantan_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBAA09A-416F-4EA3-BAA6-A369C4AD14BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD72E4C1-2FF8-4494-9E9D-000D748DA14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t># Pointers to input and output files. Paths must be relative to daily_map.py script.</t>
   </si>
@@ -76,43 +76,67 @@
     <t>data/weather_station_coords.xlsx</t>
   </si>
   <si>
+    <t>C:\Users\03125327\github\fc_hydro_kalimantan_2022\CNM_domain_creation\canal_network_graph.p</t>
+  </si>
+  <si>
+    <t>data/canal_mesh_cells.gpkg</t>
+  </si>
+  <si>
+    <t>data/best_initial_zeta.p</t>
+  </si>
+  <si>
+    <t>sourcesink</t>
+  </si>
+  <si>
+    <t>data/sourcesink.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">daily P - ET in meters for each weather station </t>
+  </si>
+  <si>
+    <t>data/reprojected_dipwells.gpkg</t>
+  </si>
+  <si>
+    <t>sensor_locations</t>
+  </si>
+  <si>
+    <t>initial_dipwell_measurements</t>
+  </si>
+  <si>
+    <t>dipwell_measurements</t>
+  </si>
+  <si>
+    <t>data/dipwell_data_from_first_rainfall_record.csv</t>
+  </si>
+  <si>
+    <t>C:\Users\03125327\Dropbox\PhD\Computation\ForestCarbon\2022 Kalimantan customer work\qgis_derivated_data\channel_net_nodes.gpkg</t>
+  </si>
+  <si>
+    <t>channel_network_nodes</t>
+  </si>
+  <si>
+    <t>C:\Users\03125327\github\fc_hydro_kalimantan_2022\data\study_area_boundary_points.gpkg</t>
+  </si>
+  <si>
+    <t>study_area_boundary_points</t>
+  </si>
+  <si>
+    <t>gmsh_geo</t>
+  </si>
+  <si>
+    <t>data/mesh/mesh.geo</t>
+  </si>
+  <si>
+    <t>channel_network_lines</t>
+  </si>
+  <si>
+    <t>C:/Users/03125327/Dropbox/PhD/Computation/ForestCarbon/2022 Kalimantan customer work/qgis_derivated_data/reprojected_canals_singleparts.gpkg</t>
+  </si>
+  <si>
+    <t>initial_condition/initial_day_dipwell_coords_and_measurements_far_from_canals.csv</t>
+  </si>
+  <si>
     <t>data/mesh/mesh_0.03.msh</t>
-  </si>
-  <si>
-    <t>C:\Users\03125327\github\fc_hydro_kalimantan_2022\CNM_domain_creation\canal_network_graph.p</t>
-  </si>
-  <si>
-    <t>data/canal_mesh_cells.gpkg</t>
-  </si>
-  <si>
-    <t>data/best_initial_zeta.p</t>
-  </si>
-  <si>
-    <t>sourcesink</t>
-  </si>
-  <si>
-    <t>data/sourcesink.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">daily P - ET in meters for each weather station </t>
-  </si>
-  <si>
-    <t>data/reprojected_dipwells.gpkg</t>
-  </si>
-  <si>
-    <t>sensor_locations</t>
-  </si>
-  <si>
-    <t>initial_dipwell_measurements</t>
-  </si>
-  <si>
-    <t>initial_condition/initial_day_dipwell_coords_and_measurements.csv</t>
-  </si>
-  <si>
-    <t>dipwell_measurements</t>
-  </si>
-  <si>
-    <t>data/dipwell_data_from_first_rainfall_record.csv</t>
   </si>
 </sst>
 </file>
@@ -482,15 +506,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" customWidth="1"/>
     <col min="2" max="2" width="93.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -541,13 +565,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -567,67 +591,99 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
+      <c r="A9" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>20</v>
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
+      <c r="A14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Before running historic rainfall data
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\fc_hydro_kalimantan_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD72E4C1-2FF8-4494-9E9D-000D748DA14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800C46F5-327B-4AB2-AEBC-54704AAC634B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3465" yWindow="3465" windowWidth="28800" windowHeight="15435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -82,15 +82,9 @@
     <t>data/canal_mesh_cells.gpkg</t>
   </si>
   <si>
-    <t>data/best_initial_zeta.p</t>
-  </si>
-  <si>
     <t>sourcesink</t>
   </si>
   <si>
-    <t>data/sourcesink.xlsx</t>
-  </si>
-  <si>
     <t xml:space="preserve">daily P - ET in meters for each weather station </t>
   </si>
   <si>
@@ -106,9 +100,6 @@
     <t>dipwell_measurements</t>
   </si>
   <si>
-    <t>data/dipwell_data_from_first_rainfall_record.csv</t>
-  </si>
-  <si>
     <t>C:\Users\03125327\Dropbox\PhD\Computation\ForestCarbon\2022 Kalimantan customer work\qgis_derivated_data\channel_net_nodes.gpkg</t>
   </si>
   <si>
@@ -137,6 +128,15 @@
   </si>
   <si>
     <t>data/mesh/mesh_0.03.msh</t>
+  </si>
+  <si>
+    <t>data/revised_dipwell_data_from_first_rainfall_record_without_canal_sensors.csv</t>
+  </si>
+  <si>
+    <t>initial_condition/best_initial_zeta.p</t>
+  </si>
+  <si>
+    <t>data/sourcesink_dry_year.xlsx</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,13 +565,13 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -592,34 +592,34 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -651,7 +651,7 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -664,26 +664,26 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added output dir location as an external variable
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t xml:space="preserve"># Pointers to input and output files. Paths must be relative to daily_map.py script.</t>
   </si>
@@ -137,6 +137,27 @@
   </si>
   <si>
     <t xml:space="preserve">data/revised_dipwell_data_from_first_rainfall_record_without_canal_sensors.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent_directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~/Programming/github/HydroTroPe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_parent_folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~/Dropbox/PhD/Computation/ForestCarbon/2022 Kalimantan customer work/0. Raw Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output_directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relative to parent_directory</t>
   </si>
 </sst>
 </file>
@@ -247,13 +268,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="93.86"/>
@@ -425,6 +446,33 @@
       </c>
       <c r="B20" s="0" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited documentation, and added description to file pointers
</commit_message>
<xml_diff>
--- a/file_pointers.xlsx
+++ b/file_pointers.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t xml:space="preserve"># Pointers to input and output files. Paths must be relative to daily_map.py script.</t>
   </si>
@@ -31,7 +31,31 @@
     <t xml:space="preserve">Path</t>
   </si>
   <si>
-    <t xml:space="preserve">Comments</t>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent_directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~/Programming/github/HydroTroPe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path to the  main directory, of which all the rest may be relative directories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_parent_folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">~/Dropbox/PhD/Computation/ForestCarbon/2022 Kalimantan customer work/0. Raw Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output_directory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">relative to parent_directory</t>
   </si>
   <si>
     <t xml:space="preserve">DEM</t>
@@ -121,6 +145,9 @@
     <t xml:space="preserve">template_output_raster</t>
   </si>
   <si>
+    <t xml:space="preserve">Raster to use as a template to output the WTD rasters. Recommended: set the same as the DEM</t>
+  </si>
+  <si>
     <t xml:space="preserve">sensor_locations</t>
   </si>
   <si>
@@ -133,31 +160,13 @@
     <t xml:space="preserve">initial_condition/initial_day_dipwell_coords_and_measurements_far_from_canals.csv</t>
   </si>
   <si>
+    <t xml:space="preserve">Necessary for the initial condition calculations</t>
+  </si>
+  <si>
     <t xml:space="preserve">dipwell_measurements</t>
   </si>
   <si>
     <t xml:space="preserve">data/revised_dipwell_data_from_first_rainfall_record_without_canal_sensors.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">parent_directory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~/Programming/github/HydroTroPe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data_parent_folder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">~/Dropbox/PhD/Computation/ForestCarbon/2022 Kalimantan customer work/0. Raw Data</t>
-  </si>
-  <si>
-    <t xml:space="preserve">output_directory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">output</t>
-  </si>
-  <si>
-    <t xml:space="preserve">relative to parent_directory</t>
   </si>
 </sst>
 </file>
@@ -268,13 +277,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="topLeft" activeCell="B32" activeCellId="0" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="35.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="93.86"/>
@@ -285,7 +294,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>1</v>
       </c>
@@ -296,7 +306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>4</v>
       </c>
@@ -307,7 +317,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>7</v>
       </c>
@@ -315,36 +325,37 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="0" t="s">
+        <v>11</v>
+      </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="C7" s="0" t="s">
+        <v>14</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="B8" s="0" t="s">
+        <v>16</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -352,129 +363,140 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="0" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="0" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
         <v>24</v>
       </c>
+      <c r="B12" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="B14" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>38</v>
+        <v>13</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>45</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>